<commit_message>
Issue 9 m07 performancetest optional (#72)
* Add temporary Excel files to .gitignore.

* Meer genuanceerde tekst.

* Files gegenereerd.
</commit_message>
<xml_diff>
--- a/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -191,14 +191,15 @@
           <t xml:space="preserve">Continuous delivery pipeline (M07)
 Er is een geautomatiseerde continuous delivery pipeline die aantoonbaar correct werkt en ten minste de volgende activiteiten uitvoert:
 - bouw van de software,
+- unit tests,
+- regressietests,
 - kwaliteitscontroles,
-- regressietests,
-- performance tests,
-- beveiligingstests,
-- unit tests,
+- performancetests (*),
+- beveiligingstests (*),
 - installatie van de software,
 - oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgever.
-De projectenorganisatie voorziet in mensen en hulpmiddelen, zodat projecten deze pipeline kunnen toepassen. Projecten zijn verantwoordelijk voor de correcte werking van de pipeline.
+(*) Idealerwijs voert de geautomatiseerde continuous delivery pipeline ook performance tests en beveiligingstests uit. Vanwege de doorlooptijden van tests (met name van duurtesten) en licenties van testtools is dat niet altijd haalbaar. In dat geval vinden de performance tests en beveiligingstests periodiek en zo vaak mogelijk plaats, bij voorkeur dagelijks.
+De projectenorganisatie voorziet in mensen en hulpmiddelen, zodat projecten deze pipeline kunnen toepassen. Projecten zijn verantwoordelijk voor de correcte werking van de pipelin.
 Rationale
 Software incrementeel opleveren (zie [M05: Iteratief en incrementeel ontwikkelproces](#iteratief-en-incrementeel-ontwikkelproces-m05-)) vereist dat de software frequent gebouwd, getest en opgeleverd kan worden. Om dit efficiënt en foutvrij te doen, dient het proces van bouwen, testen en opleveren geautomatiseerd te zijn; een continuous delivery pipeline faciliteert dit.
 ICTU
@@ -581,9 +582,9 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Periodieke beoordeling informatiebeveiliging (M26)
-Projecten laten periodiek een beveiligingstest uitvoeren. De code wordt zowel geautomatiseerd, als handmatig onderzocht op veelvoorkomende kwetsbaarheden door een beveiligingsexpert van buiten het project. De projectorganisatie zorgt ervoor dat deze expertise op afroep beschikbaar gesteld wordt aan projecten. Bevindingen uit de beveiligingstest worden vastgelegd als onderdeel van de werkvoorraad voor het ontwikkelproces (zie [M05: Iteratief en incrementeel ontwikkelproces](#iteratief-en-incrementeel-ontwikkelproces-m05-)).
-Rationale
-Door het inschakelen van actuele, specifieke expertise wordt de kans vergroot dat eventuele kwetsbaarheden in de gerealiseerde software tijdig herkend worden. Doordat de projectenorganisatie deze expertise beschikbaar stelt, kunnen projecten daar snel en efficiënt gebruik van maken.
+Projecten laten periodiek een beveiligingstest uitvoeren. De code wordt zowel geautomatiseerd, als handmatig onderzocht op veelvoorkomende kwetsbaarheden door een beveiligingsexpert van buiten het project. Bevindingen uit de beveiligingstest worden vastgelegd als onderdeel van de werkvoorraad voor het ontwikkelproces (zie [M05: Iteratief en incrementeel ontwikkelproces](#iteratief-en-incrementeel-ontwikkelproces-m05-)).
+Rationale
+Door het inschakelen van actuele, specifieke expertise wordt de kans vergroot dat eventuele kwetsbaarheden in de gerealiseerde software tijdig herkend worden.
 ICTU
 Software wordt minimaal bij iedere grote release of tenminste twee keer per jaar onderworpen aan een beveiligingstest door beveiligingsexperts die ICTU daarvoor inhuurt. Op basis van documentatie en architectuurstudie, crystalbox security audits (broncodescan) en penetratieaudits beoordelen deze experts of de software voldoet aan de projectspecifieke niet-functionele eisen met betrekking tot beveiliging, of bekende kwetsbaarheden (OWASP) vermeden zijn en in hoeverre voldoende invulling gegeven is aan de normen vanuit die vanuit BIR en SSD gelden.
 Indien door de opdrachtgever gewenst kunnen securitytesten door een onafhankelijke derde partij worden uitgevoerd in een daarvoor door de opdrachtgever beschikbaar gestelde omgeving. Dit kan zowel incidenteel als structureel worden ingericht. Afspraken hierover worden bij voorkeur al in de voorbereidingsfase gemaakt.
@@ -637,7 +638,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.1.287, 23-06-2018.</t>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.1.288, 12-07-2018.</t>
   </si>
   <si>
     <t>Maatregel</t>
@@ -754,19 +755,19 @@
     <t>1. bouw van de software</t>
   </si>
   <si>
-    <t>2. kwaliteitscontroles</t>
+    <t>2. unit tests</t>
   </si>
   <si>
     <t>3. regressietests</t>
   </si>
   <si>
-    <t>4. performance tests</t>
-  </si>
-  <si>
-    <t>5. beveiligingstests</t>
-  </si>
-  <si>
-    <t>6. unit tests</t>
+    <t>4. kwaliteitscontroles</t>
+  </si>
+  <si>
+    <t>5. performancetests (*)</t>
+  </si>
+  <si>
+    <t>6. beveiligingstests (*)</t>
   </si>
   <si>
     <t>7. installatie van de software</t>

</xml_diff>

<commit_message>
Expand M05 in checklist.
</commit_message>
<xml_diff>
--- a/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -206,7 +206,7 @@
 ICTU
 ICTU gebruikt hiervoor Scrum, een raamwerk voor agile productontwikkeling. ICTU propageert de kernwaarden van Scrum en vereist de volgende onderdelen van Scrum:
 - Scrum team bestaand uit product owner, ontwikkelteam en Scrum master,
-- Proces: daily scrum, sprints, sprint planning, sprint review, sprint refinement,
+- Proces met daily scrum, sprints, sprint planning, sprint review, sprint refinement,
 - Definition of Done,
 - Definition of Ready,
 - Product backlog.
@@ -215,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B31" authorId="0">
+    <comment ref="B36" authorId="0">
       <text>
         <r>
           <rPr>
@@ -234,7 +234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B32" authorId="0">
+    <comment ref="B37" authorId="0">
       <text>
         <r>
           <rPr>
@@ -263,7 +263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B41" authorId="0">
+    <comment ref="B46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -282,7 +282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B42" authorId="0">
+    <comment ref="B47" authorId="0">
       <text>
         <r>
           <rPr>
@@ -297,8 +297,8 @@
 Voor de belangrijkste verschillen beschrijft de projectverantwoordelijke:
 - het geconstateerde verschil,
 - reden voor het verschil,
-- in geval van acceptatie: waarom het verschil geaccepteerd wordt,
-- in geval van verbeteractie: planning om het verschil weg te werken.
+- in geval van acceptatie; waarom het verschil geaccepteerd wordt,
+- in geval van verbeteractie; planning om het verschil weg te werken.
 Rationale
 De implementatie van een nieuwe versie van de kwaliteitsaanpak kost tijd. De introductie en aanpassing van normen en tools, kunnen verschillende consequenties hebben: bestaande broncode blijkt niet meer volledig te voldoen aan de normen, een nieuwe tool moet in de ontwikkelstraat worden toegevoegd, enzovoort.
 Anderzijds is het voor de uniformiteit van kwaliteitsmeting en rapportage en de doorontwikkeling van de kwaliteitsaanpak van belang de implementatieperiode zo kort mogelijk en voorspelbaar te houden. Daarom stemt de projectenorganisatie met de projecten een implementatiemoment en implementatieperiode af.
@@ -309,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B43" authorId="0">
+    <comment ref="B48" authorId="0">
       <text>
         <r>
           <rPr>
@@ -336,7 +336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B44" authorId="0">
+    <comment ref="B49" authorId="0">
       <text>
         <r>
           <rPr>
@@ -355,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B45" authorId="0">
+    <comment ref="B50" authorId="0">
       <text>
         <r>
           <rPr>
@@ -374,7 +374,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B47" authorId="0">
+    <comment ref="B52" authorId="0">
       <text>
         <r>
           <rPr>
@@ -405,7 +405,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B48" authorId="0">
+    <comment ref="B53" authorId="0">
       <text>
         <r>
           <rPr>
@@ -432,7 +432,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B49" authorId="0">
+    <comment ref="B54" authorId="0">
       <text>
         <r>
           <rPr>
@@ -452,7 +452,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B50" authorId="0">
+    <comment ref="B55" authorId="0">
       <text>
         <r>
           <rPr>
@@ -472,7 +472,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B51" authorId="0">
+    <comment ref="B56" authorId="0">
       <text>
         <r>
           <rPr>
@@ -491,7 +491,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B52" authorId="0">
+    <comment ref="B57" authorId="0">
       <text>
         <r>
           <rPr>
@@ -528,7 +528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B62" authorId="0">
+    <comment ref="B67" authorId="0">
       <text>
         <r>
           <rPr>
@@ -554,7 +554,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B66" authorId="0">
+    <comment ref="B71" authorId="0">
       <text>
         <r>
           <rPr>
@@ -573,7 +573,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B67" authorId="0">
+    <comment ref="B72" authorId="0">
       <text>
         <r>
           <rPr>
@@ -592,7 +592,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B68" authorId="0">
+    <comment ref="B73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -609,7 +609,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B69" authorId="0">
+    <comment ref="B74" authorId="0">
       <text>
         <r>
           <rPr>
@@ -628,7 +628,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B70" authorId="0">
+    <comment ref="B75" authorId="0">
       <text>
         <r>
           <rPr>
@@ -650,9 +650,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
-  <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.1.515, 30-07-2018.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+  <si>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.1.710, 31-07-2018.</t>
   </si>
   <si>
     <t>Maatregel</t>
@@ -772,6 +772,21 @@
     <t>Iteratief en incrementeel ontwikkelproces</t>
   </si>
   <si>
+    <t>1. Scrum team bestaand uit product owner, ontwikkelteam en Scrum master</t>
+  </si>
+  <si>
+    <t>2. Proces met daily scrum, sprints, sprint planning, sprint review, sprint refinement</t>
+  </si>
+  <si>
+    <t>3. Definition of Done</t>
+  </si>
+  <si>
+    <t>4. Definition of Ready</t>
+  </si>
+  <si>
+    <t>5. Product backlog</t>
+  </si>
+  <si>
     <t>M06</t>
   </si>
   <si>
@@ -805,7 +820,7 @@
     <t>7. installatie van de software</t>
   </si>
   <si>
-    <t>8. oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgever.</t>
+    <t>8. oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgever</t>
   </si>
   <si>
     <t>M08</t>
@@ -1368,7 +1383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
@@ -1646,29 +1661,25 @@
       <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="7"/>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="4"/>
+      <c r="C32" s="7"/>
       <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="6"/>
       <c r="B33" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="5"/>
@@ -1676,7 +1687,7 @@
     <row r="34" spans="1:4">
       <c r="A34" s="6"/>
       <c r="B34" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="5"/>
@@ -1684,25 +1695,29 @@
     <row r="35" spans="1:4">
       <c r="A35" s="6"/>
       <c r="B35" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6" t="s">
+      <c r="A36" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="7"/>
+      <c r="C37" s="4"/>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4">
@@ -1730,161 +1745,161 @@
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="7"/>
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="5"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="3" t="s">
+      <c r="C42" s="7"/>
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="C43" s="7"/>
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="5"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="3" t="s">
+      <c r="C44" s="7"/>
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="C45" s="7"/>
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="5"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="5"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="5"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="5"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C51" s="4"/>
-      <c r="D51" s="5"/>
+      <c r="A51" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="5"/>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6" t="s">
+      <c r="A53" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" s="4"/>
+      <c r="D53" s="5"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C54" s="4"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="7"/>
-      <c r="D53" s="5"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6" t="s">
+      <c r="C55" s="4"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C54" s="7"/>
-      <c r="D54" s="5"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6" t="s">
+      <c r="B56" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C55" s="7"/>
-      <c r="D55" s="5"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6" t="s">
+      <c r="C56" s="4"/>
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C56" s="7"/>
-      <c r="D56" s="5"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="6"/>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C57" s="7"/>
+      <c r="C57" s="4"/>
       <c r="D57" s="5"/>
     </row>
     <row r="58" spans="1:4">
@@ -1920,19 +1935,17 @@
       <c r="D61" s="5"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="6"/>
+      <c r="B62" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C62" s="4"/>
+      <c r="C62" s="7"/>
       <c r="D62" s="5"/>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="6"/>
       <c r="B63" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C63" s="7"/>
       <c r="D63" s="5"/>
@@ -1940,7 +1953,7 @@
     <row r="64" spans="1:4">
       <c r="A64" s="6"/>
       <c r="B64" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="5"/>
@@ -1948,69 +1961,111 @@
     <row r="65" spans="1:4">
       <c r="A65" s="6"/>
       <c r="B65" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="5"/>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C66" s="4"/>
+      <c r="A66" s="6"/>
+      <c r="B66" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" s="7"/>
       <c r="D66" s="5"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="5"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="6"/>
+      <c r="B68" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" s="7"/>
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="6"/>
+      <c r="B69" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C69" s="7"/>
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="6"/>
+      <c r="B70" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="C70" s="7"/>
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C68" s="4"/>
-      <c r="D68" s="5"/>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="3" t="s">
+      <c r="B71" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="C71" s="4"/>
+      <c r="D71" s="5"/>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C69" s="4"/>
-      <c r="D69" s="5"/>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="3" t="s">
+      <c r="B72" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="C72" s="4"/>
+      <c r="D72" s="5"/>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C70" s="4"/>
-      <c r="D70" s="5"/>
+      <c r="B73" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C73" s="4"/>
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C74" s="4"/>
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C75" s="4"/>
+      <c r="D75" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A51:D51"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C72">
+  <conditionalFormatting sqref="C3:C77">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2025,7 +2080,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C72">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C77">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Expand M05 in checklist. (#86)
</commit_message>
<xml_diff>
--- a/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -206,7 +206,7 @@
 ICTU
 ICTU gebruikt hiervoor Scrum, een raamwerk voor agile productontwikkeling. ICTU propageert de kernwaarden van Scrum en vereist de volgende onderdelen van Scrum:
 - Scrum team bestaand uit product owner, ontwikkelteam en Scrum master,
-- Proces: daily scrum, sprints, sprint planning, sprint review, sprint refinement,
+- Proces met daily scrum, sprints, sprint planning, sprint review, sprint refinement,
 - Definition of Done,
 - Definition of Ready,
 - Product backlog.
@@ -215,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B31" authorId="0">
+    <comment ref="B36" authorId="0">
       <text>
         <r>
           <rPr>
@@ -234,7 +234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B32" authorId="0">
+    <comment ref="B37" authorId="0">
       <text>
         <r>
           <rPr>
@@ -263,7 +263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B41" authorId="0">
+    <comment ref="B46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -282,7 +282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B42" authorId="0">
+    <comment ref="B47" authorId="0">
       <text>
         <r>
           <rPr>
@@ -297,8 +297,8 @@
 Voor de belangrijkste verschillen beschrijft de projectverantwoordelijke:
 - het geconstateerde verschil,
 - reden voor het verschil,
-- in geval van acceptatie: waarom het verschil geaccepteerd wordt,
-- in geval van verbeteractie: planning om het verschil weg te werken.
+- in geval van acceptatie; waarom het verschil geaccepteerd wordt,
+- in geval van verbeteractie; planning om het verschil weg te werken.
 Rationale
 De implementatie van een nieuwe versie van de kwaliteitsaanpak kost tijd. De introductie en aanpassing van normen en tools, kunnen verschillende consequenties hebben: bestaande broncode blijkt niet meer volledig te voldoen aan de normen, een nieuwe tool moet in de ontwikkelstraat worden toegevoegd, enzovoort.
 Anderzijds is het voor de uniformiteit van kwaliteitsmeting en rapportage en de doorontwikkeling van de kwaliteitsaanpak van belang de implementatieperiode zo kort mogelijk en voorspelbaar te houden. Daarom stemt de projectenorganisatie met de projecten een implementatiemoment en implementatieperiode af.
@@ -309,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B43" authorId="0">
+    <comment ref="B48" authorId="0">
       <text>
         <r>
           <rPr>
@@ -336,7 +336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B44" authorId="0">
+    <comment ref="B49" authorId="0">
       <text>
         <r>
           <rPr>
@@ -355,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B45" authorId="0">
+    <comment ref="B50" authorId="0">
       <text>
         <r>
           <rPr>
@@ -374,7 +374,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B47" authorId="0">
+    <comment ref="B52" authorId="0">
       <text>
         <r>
           <rPr>
@@ -405,7 +405,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B48" authorId="0">
+    <comment ref="B53" authorId="0">
       <text>
         <r>
           <rPr>
@@ -432,7 +432,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B49" authorId="0">
+    <comment ref="B54" authorId="0">
       <text>
         <r>
           <rPr>
@@ -452,7 +452,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B50" authorId="0">
+    <comment ref="B55" authorId="0">
       <text>
         <r>
           <rPr>
@@ -472,7 +472,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B51" authorId="0">
+    <comment ref="B56" authorId="0">
       <text>
         <r>
           <rPr>
@@ -491,7 +491,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B52" authorId="0">
+    <comment ref="B57" authorId="0">
       <text>
         <r>
           <rPr>
@@ -528,7 +528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B62" authorId="0">
+    <comment ref="B67" authorId="0">
       <text>
         <r>
           <rPr>
@@ -554,7 +554,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B66" authorId="0">
+    <comment ref="B71" authorId="0">
       <text>
         <r>
           <rPr>
@@ -573,7 +573,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B67" authorId="0">
+    <comment ref="B72" authorId="0">
       <text>
         <r>
           <rPr>
@@ -592,7 +592,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B68" authorId="0">
+    <comment ref="B73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -609,7 +609,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B69" authorId="0">
+    <comment ref="B74" authorId="0">
       <text>
         <r>
           <rPr>
@@ -628,7 +628,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B70" authorId="0">
+    <comment ref="B75" authorId="0">
       <text>
         <r>
           <rPr>
@@ -650,9 +650,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
-  <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.1.515, 30-07-2018.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+  <si>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.1.710, 31-07-2018.</t>
   </si>
   <si>
     <t>Maatregel</t>
@@ -772,6 +772,21 @@
     <t>Iteratief en incrementeel ontwikkelproces</t>
   </si>
   <si>
+    <t>1. Scrum team bestaand uit product owner, ontwikkelteam en Scrum master</t>
+  </si>
+  <si>
+    <t>2. Proces met daily scrum, sprints, sprint planning, sprint review, sprint refinement</t>
+  </si>
+  <si>
+    <t>3. Definition of Done</t>
+  </si>
+  <si>
+    <t>4. Definition of Ready</t>
+  </si>
+  <si>
+    <t>5. Product backlog</t>
+  </si>
+  <si>
     <t>M06</t>
   </si>
   <si>
@@ -805,7 +820,7 @@
     <t>7. installatie van de software</t>
   </si>
   <si>
-    <t>8. oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgever.</t>
+    <t>8. oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgever</t>
   </si>
   <si>
     <t>M08</t>
@@ -1368,7 +1383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
@@ -1646,29 +1661,25 @@
       <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="7"/>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="4"/>
+      <c r="C32" s="7"/>
       <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="6"/>
       <c r="B33" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="5"/>
@@ -1676,7 +1687,7 @@
     <row r="34" spans="1:4">
       <c r="A34" s="6"/>
       <c r="B34" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="5"/>
@@ -1684,25 +1695,29 @@
     <row r="35" spans="1:4">
       <c r="A35" s="6"/>
       <c r="B35" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6" t="s">
+      <c r="A36" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="7"/>
+      <c r="C37" s="4"/>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4">
@@ -1730,161 +1745,161 @@
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="7"/>
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="5"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="3" t="s">
+      <c r="C42" s="7"/>
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="C43" s="7"/>
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="5"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="3" t="s">
+      <c r="C44" s="7"/>
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="C45" s="7"/>
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="5"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="5"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="5"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="5"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C51" s="4"/>
-      <c r="D51" s="5"/>
+      <c r="A51" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="5"/>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6" t="s">
+      <c r="A53" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" s="4"/>
+      <c r="D53" s="5"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C54" s="4"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="7"/>
-      <c r="D53" s="5"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6" t="s">
+      <c r="C55" s="4"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C54" s="7"/>
-      <c r="D54" s="5"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6" t="s">
+      <c r="B56" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C55" s="7"/>
-      <c r="D55" s="5"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6" t="s">
+      <c r="C56" s="4"/>
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C56" s="7"/>
-      <c r="D56" s="5"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="6"/>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C57" s="7"/>
+      <c r="C57" s="4"/>
       <c r="D57" s="5"/>
     </row>
     <row r="58" spans="1:4">
@@ -1920,19 +1935,17 @@
       <c r="D61" s="5"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="6"/>
+      <c r="B62" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C62" s="4"/>
+      <c r="C62" s="7"/>
       <c r="D62" s="5"/>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="6"/>
       <c r="B63" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C63" s="7"/>
       <c r="D63" s="5"/>
@@ -1940,7 +1953,7 @@
     <row r="64" spans="1:4">
       <c r="A64" s="6"/>
       <c r="B64" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="5"/>
@@ -1948,69 +1961,111 @@
     <row r="65" spans="1:4">
       <c r="A65" s="6"/>
       <c r="B65" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="5"/>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C66" s="4"/>
+      <c r="A66" s="6"/>
+      <c r="B66" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" s="7"/>
       <c r="D66" s="5"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="5"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="6"/>
+      <c r="B68" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" s="7"/>
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="6"/>
+      <c r="B69" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C69" s="7"/>
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="6"/>
+      <c r="B70" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="C70" s="7"/>
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C68" s="4"/>
-      <c r="D68" s="5"/>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="3" t="s">
+      <c r="B71" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="C71" s="4"/>
+      <c r="D71" s="5"/>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C69" s="4"/>
-      <c r="D69" s="5"/>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="3" t="s">
+      <c r="B72" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="C72" s="4"/>
+      <c r="D72" s="5"/>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C70" s="4"/>
-      <c r="D70" s="5"/>
+      <c r="B73" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C73" s="4"/>
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C74" s="4"/>
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C75" s="4"/>
+      <c r="D75" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A51:D51"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C72">
+  <conditionalFormatting sqref="C3:C77">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2025,7 +2080,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C72">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C77">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add missing Scrum terms. Fixed #90.
</commit_message>
<xml_diff>
--- a/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -206,16 +206,15 @@
 ICTU
 ICTU gebruikt hiervoor Scrum, een raamwerk voor agile productontwikkeling. ICTU propageert de kernwaarden van Scrum en vereist de volgende onderdelen van Scrum:
 - Scrum team bestaand uit product owner, ontwikkelteam en Scrum master,
-- Proces met daily scrum, sprints, sprint planning, sprint review, sprint refinement,
-- Definition of Done,
-- Definition of Ready,
-- Product backlog.
+- Proces met daily scrum, sprints, sprint planning, sprint review, sprint retrospective en sprint refinement,
+- Definition of Ready en Definition of Done,
+- Product backlog en sprint backlog.
 Vast onderdeel van de Definition of Done is dat producten actueel en onderling consistent zijn ([M01: Op te leveren producten](#op-te-leveren-producten-m01-)) en voldoen aan de door de projectenorganisatie vastgestelde kwaliteitsnormen ([M02: Continu voldoen aan kwaliteitsnormen](#continu-voldoen-aan-kwaliteitsnormen-m02-)).
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B36" authorId="0">
+    <comment ref="B35" authorId="0">
       <text>
         <r>
           <rPr>
@@ -234,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B37" authorId="0">
+    <comment ref="B36" authorId="0">
       <text>
         <r>
           <rPr>
@@ -263,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B46" authorId="0">
+    <comment ref="B45" authorId="0">
       <text>
         <r>
           <rPr>
@@ -282,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B47" authorId="0">
+    <comment ref="B46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -309,7 +308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B48" authorId="0">
+    <comment ref="B47" authorId="0">
       <text>
         <r>
           <rPr>
@@ -336,7 +335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B49" authorId="0">
+    <comment ref="B48" authorId="0">
       <text>
         <r>
           <rPr>
@@ -355,7 +354,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B50" authorId="0">
+    <comment ref="B49" authorId="0">
       <text>
         <r>
           <rPr>
@@ -374,7 +373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B52" authorId="0">
+    <comment ref="B51" authorId="0">
       <text>
         <r>
           <rPr>
@@ -405,7 +404,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B53" authorId="0">
+    <comment ref="B52" authorId="0">
       <text>
         <r>
           <rPr>
@@ -432,7 +431,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B54" authorId="0">
+    <comment ref="B53" authorId="0">
       <text>
         <r>
           <rPr>
@@ -452,7 +451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B55" authorId="0">
+    <comment ref="B54" authorId="0">
       <text>
         <r>
           <rPr>
@@ -472,7 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B56" authorId="0">
+    <comment ref="B55" authorId="0">
       <text>
         <r>
           <rPr>
@@ -491,7 +490,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B57" authorId="0">
+    <comment ref="B56" authorId="0">
       <text>
         <r>
           <rPr>
@@ -528,7 +527,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B67" authorId="0">
+    <comment ref="B66" authorId="0">
       <text>
         <r>
           <rPr>
@@ -554,7 +553,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B71" authorId="0">
+    <comment ref="B70" authorId="0">
       <text>
         <r>
           <rPr>
@@ -573,7 +572,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B72" authorId="0">
+    <comment ref="B71" authorId="0">
       <text>
         <r>
           <rPr>
@@ -592,7 +591,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B73" authorId="0">
+    <comment ref="B72" authorId="0">
       <text>
         <r>
           <rPr>
@@ -609,7 +608,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B74" authorId="0">
+    <comment ref="B73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -628,7 +627,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B75" authorId="0">
+    <comment ref="B74" authorId="0">
       <text>
         <r>
           <rPr>
@@ -650,9 +649,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
-  <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.2.0-build.5, 01-08-2018.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+  <si>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.2.1-build.1, 29-08-2018.</t>
   </si>
   <si>
     <t>Maatregel</t>
@@ -775,16 +774,13 @@
     <t>1. Scrum team bestaand uit product owner, ontwikkelteam en Scrum master</t>
   </si>
   <si>
-    <t>2. Proces met daily scrum, sprints, sprint planning, sprint review, sprint refinement</t>
-  </si>
-  <si>
-    <t>3. Definition of Done</t>
-  </si>
-  <si>
-    <t>4. Definition of Ready</t>
-  </si>
-  <si>
-    <t>5. Product backlog</t>
+    <t>2. Proces met daily scrum, sprints, sprint planning, sprint review, sprint retrospective en sprint refinement</t>
+  </si>
+  <si>
+    <t>3. Definition of Ready en Definition of Done</t>
+  </si>
+  <si>
+    <t>4. Product backlog en sprint backlog</t>
   </si>
   <si>
     <t>M06</t>
@@ -1383,7 +1379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
@@ -1693,31 +1689,31 @@
       <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6" t="s">
+      <c r="A35" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="7"/>
+      <c r="B35" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="4"/>
       <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="3" t="s">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="4"/>
+      <c r="C37" s="7"/>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4">
@@ -1777,129 +1773,129 @@
       <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6" t="s">
+      <c r="A45" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="7"/>
+      <c r="B45" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="4"/>
       <c r="D45" s="5"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="5"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="5"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B50" s="3" t="s">
+      <c r="A50" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C50" s="4"/>
-      <c r="D50" s="5"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+      <c r="B51" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" s="4"/>
+      <c r="D51" s="5"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="5"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="5"/>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B57" s="3" t="s">
+      <c r="A57" s="6"/>
+      <c r="B57" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C57" s="4"/>
+      <c r="C57" s="7"/>
       <c r="D57" s="5"/>
     </row>
     <row r="58" spans="1:4">
@@ -1967,21 +1963,21 @@
       <c r="D65" s="5"/>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="6"/>
-      <c r="B66" s="6" t="s">
+      <c r="A66" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C66" s="7"/>
+      <c r="B66" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C66" s="4"/>
       <c r="D66" s="5"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B67" s="3" t="s">
+      <c r="A67" s="6"/>
+      <c r="B67" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C67" s="4"/>
+      <c r="C67" s="7"/>
       <c r="D67" s="5"/>
     </row>
     <row r="68" spans="1:4">
@@ -2001,71 +1997,63 @@
       <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="6"/>
-      <c r="B70" s="6" t="s">
+      <c r="A70" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C70" s="7"/>
+      <c r="B70" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C70" s="4"/>
       <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="5"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="5"/>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C73" s="4"/>
       <c r="D73" s="5"/>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C74" s="4"/>
       <c r="D74" s="5"/>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C75" s="4"/>
-      <c r="D75" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A50:D50"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C77">
+  <conditionalFormatting sqref="C3:C76">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2080,7 +2068,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C77">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C76">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add missing Scrum terms. Fixed #90. (#92)
</commit_message>
<xml_diff>
--- a/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -206,16 +206,15 @@
 ICTU
 ICTU gebruikt hiervoor Scrum, een raamwerk voor agile productontwikkeling. ICTU propageert de kernwaarden van Scrum en vereist de volgende onderdelen van Scrum:
 - Scrum team bestaand uit product owner, ontwikkelteam en Scrum master,
-- Proces met daily scrum, sprints, sprint planning, sprint review, sprint refinement,
-- Definition of Done,
-- Definition of Ready,
-- Product backlog.
+- Proces met daily scrum, sprints, sprint planning, sprint review, sprint retrospective en sprint refinement,
+- Definition of Ready en Definition of Done,
+- Product backlog en sprint backlog.
 Vast onderdeel van de Definition of Done is dat producten actueel en onderling consistent zijn ([M01: Op te leveren producten](#op-te-leveren-producten-m01-)) en voldoen aan de door de projectenorganisatie vastgestelde kwaliteitsnormen ([M02: Continu voldoen aan kwaliteitsnormen](#continu-voldoen-aan-kwaliteitsnormen-m02-)).
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B36" authorId="0">
+    <comment ref="B35" authorId="0">
       <text>
         <r>
           <rPr>
@@ -234,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B37" authorId="0">
+    <comment ref="B36" authorId="0">
       <text>
         <r>
           <rPr>
@@ -263,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B46" authorId="0">
+    <comment ref="B45" authorId="0">
       <text>
         <r>
           <rPr>
@@ -282,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B47" authorId="0">
+    <comment ref="B46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -309,7 +308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B48" authorId="0">
+    <comment ref="B47" authorId="0">
       <text>
         <r>
           <rPr>
@@ -336,7 +335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B49" authorId="0">
+    <comment ref="B48" authorId="0">
       <text>
         <r>
           <rPr>
@@ -355,7 +354,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B50" authorId="0">
+    <comment ref="B49" authorId="0">
       <text>
         <r>
           <rPr>
@@ -374,7 +373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B52" authorId="0">
+    <comment ref="B51" authorId="0">
       <text>
         <r>
           <rPr>
@@ -405,7 +404,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B53" authorId="0">
+    <comment ref="B52" authorId="0">
       <text>
         <r>
           <rPr>
@@ -432,7 +431,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B54" authorId="0">
+    <comment ref="B53" authorId="0">
       <text>
         <r>
           <rPr>
@@ -452,7 +451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B55" authorId="0">
+    <comment ref="B54" authorId="0">
       <text>
         <r>
           <rPr>
@@ -472,7 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B56" authorId="0">
+    <comment ref="B55" authorId="0">
       <text>
         <r>
           <rPr>
@@ -491,7 +490,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B57" authorId="0">
+    <comment ref="B56" authorId="0">
       <text>
         <r>
           <rPr>
@@ -528,7 +527,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B67" authorId="0">
+    <comment ref="B66" authorId="0">
       <text>
         <r>
           <rPr>
@@ -554,7 +553,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B71" authorId="0">
+    <comment ref="B70" authorId="0">
       <text>
         <r>
           <rPr>
@@ -573,7 +572,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B72" authorId="0">
+    <comment ref="B71" authorId="0">
       <text>
         <r>
           <rPr>
@@ -592,7 +591,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B73" authorId="0">
+    <comment ref="B72" authorId="0">
       <text>
         <r>
           <rPr>
@@ -609,7 +608,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B74" authorId="0">
+    <comment ref="B73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -628,7 +627,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B75" authorId="0">
+    <comment ref="B74" authorId="0">
       <text>
         <r>
           <rPr>
@@ -650,9 +649,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
-  <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.2.0-build.5, 01-08-2018.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+  <si>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.2.1-build.1, 29-08-2018.</t>
   </si>
   <si>
     <t>Maatregel</t>
@@ -775,16 +774,13 @@
     <t>1. Scrum team bestaand uit product owner, ontwikkelteam en Scrum master</t>
   </si>
   <si>
-    <t>2. Proces met daily scrum, sprints, sprint planning, sprint review, sprint refinement</t>
-  </si>
-  <si>
-    <t>3. Definition of Done</t>
-  </si>
-  <si>
-    <t>4. Definition of Ready</t>
-  </si>
-  <si>
-    <t>5. Product backlog</t>
+    <t>2. Proces met daily scrum, sprints, sprint planning, sprint review, sprint retrospective en sprint refinement</t>
+  </si>
+  <si>
+    <t>3. Definition of Ready en Definition of Done</t>
+  </si>
+  <si>
+    <t>4. Product backlog en sprint backlog</t>
   </si>
   <si>
     <t>M06</t>
@@ -1383,7 +1379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
@@ -1693,31 +1689,31 @@
       <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6" t="s">
+      <c r="A35" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="7"/>
+      <c r="B35" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="4"/>
       <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="3" t="s">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="4"/>
+      <c r="C37" s="7"/>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4">
@@ -1777,129 +1773,129 @@
       <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6" t="s">
+      <c r="A45" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="7"/>
+      <c r="B45" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="4"/>
       <c r="D45" s="5"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="5"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="5"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B50" s="3" t="s">
+      <c r="A50" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C50" s="4"/>
-      <c r="D50" s="5"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+      <c r="B51" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" s="4"/>
+      <c r="D51" s="5"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="5"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="5"/>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B57" s="3" t="s">
+      <c r="A57" s="6"/>
+      <c r="B57" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C57" s="4"/>
+      <c r="C57" s="7"/>
       <c r="D57" s="5"/>
     </row>
     <row r="58" spans="1:4">
@@ -1967,21 +1963,21 @@
       <c r="D65" s="5"/>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="6"/>
-      <c r="B66" s="6" t="s">
+      <c r="A66" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C66" s="7"/>
+      <c r="B66" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C66" s="4"/>
       <c r="D66" s="5"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B67" s="3" t="s">
+      <c r="A67" s="6"/>
+      <c r="B67" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C67" s="4"/>
+      <c r="C67" s="7"/>
       <c r="D67" s="5"/>
     </row>
     <row r="68" spans="1:4">
@@ -2001,71 +1997,63 @@
       <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="6"/>
-      <c r="B70" s="6" t="s">
+      <c r="A70" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C70" s="7"/>
+      <c r="B70" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C70" s="4"/>
       <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="5"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="5"/>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C73" s="4"/>
       <c r="D73" s="5"/>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C74" s="4"/>
       <c r="D74" s="5"/>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C75" s="4"/>
-      <c r="D75" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A50:D50"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C77">
+  <conditionalFormatting sqref="C3:C76">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2080,7 +2068,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C77">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C76">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Generate appendix with abbreviations.
</commit_message>
<xml_diff>
--- a/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -44,10 +44,10 @@
           <t xml:space="preserve">Op te leveren producten (M01)
 Projecten zijn gesplitst in een voorbereidingsfase en een realisatiefase (zie [M14: Projecten splitsen in een voorbereidingsfase en een realisatiefase](#projecten-splitsen-in-een-voorbereidingsfase-en-een-realisatiefase-m14-)); alle fasen kennen specifieke producten. De onderstaande tabel benoemt de producten die een project in die fasen moet realiseren of waarover het project moet kunnen beschikken, indien er andere auteurs zijn (bijvoorbeeld de opdrachtgever). Het project zorgt voor een volledige oplevering van alle genoemde producten, waaronder de producten die niet door het project zelf zijn gemaakt.
 Als tijdens een project bestaande software dient te worden afgebouwd, onderhouden en/of herbouwd, vindt een onderzoek plaats naar de compleetheid en consistentie van de bestaande softwareproducten aan de hand van de onderstaande tabel (inclusief de deliverables in de kolom 'Realisatiefase') en wordt de kwaliteit van de bestaande software-producten getoetst ([M02: Continu voldoen aan kwaliteitsnormen](#continu-voldoen-aan-kwaliteitsnormen-m02-)). Dit onderzoek is onderdeel van de voorbereidingsfase en wordt uitgevoerd door vertegenwoordigers van de projectenorganisatie en medewerkers van het desbetreffende project.
-| Product                 | Voorbereidings᠆fase  | Voorbereidings᠆fase met onderzoek  | Realisatie᠆fase |
+| Product                | Voorbereidings᠆fase  | Voorbereidings᠆fase met onderzoek  | Realisatie᠆fase |
 |----------------------------------------------------------------------------------------|---|---|---|
-| Business impact analysis (BIA)*                                                        | ✔ | ✔ | ✔ |
-| Privacy impact analysis (PIA)**                                                        | ✔ | ✔ | ✔ |
+| BIA (Business impact analysis)*                                                        | ✔ | ✔ | ✔ |
+| PIA (Privacy impact analysis)**                                                        | ✔ | ✔ | ✔ |
 | Beschrijving van functionele eisen                                                     | ✔ | ✔ | ✔ |
 | Beschrijving van niet-functionele eisen                                                | ✔ | ✔ | ✔ |
 | Ontwerp- en architectuurdocumentatie (software, interactie, infrastructuur)            | ✔ | ✔ | ✔ |
@@ -76,11 +76,11 @@
 In een PIA legt de vragende organisatie vast wat de privacy-gevoeligheid is van de gegevens die in een proces of systeem worden verzameld en verwerkt. Zicht op privacygevoelige gegevens en het (laten) treffen van adequate en afdoende beschermingsmaatregelen is een wettelijke plicht die een organisatie niet aan een andere partij kan verdragen.
 ICTU
 ICTU hanteert de volgende documenten, templates en documentstandaarden voor softwarerealisatieprojecten:
-- De beschrijving van niet-functionele eisen is gebaseerd op ISO-25010, BIR en SSD, en bevat een prioritering van de niet-functionele eisen. De beschrijving van niet-functionele eisen is gebaseerd op het ICTU NFE-template. De beschrijving bevat in ieder geval eisen aan toegangsbeveiliging, aan beheerfuncties, aan logging en aan het gewenste gedrag van de software bij uitval van infrastructurele diensten, zoals een log-server;
+- De beschrijving van niet-functionele eisen is gebaseerd op ISO (International Organization for Standardization)-25010, de BIR (Baseline Informatiebeveiliging Rijksdienst) en de methode Grip op SSD (Secure software development) van het CIP (Centrum Informatiebeveiliging en Privacybescherming), en bevat een prioritering van de niet-functionele eisen. De beschrijving van niet-functionele eisen is gebaseerd op het ICTU NFE (Niet-functionele eisen)-template. De beschrijving bevat in ieder geval eisen aan toegangsbeveiliging, aan beheerfuncties, aan logging en aan het gewenste gedrag van de software bij uitval van infrastructurele diensten, zoals een log-server;
 - De beschrijving van functionele eisen bestaat uit een geprioriteerde backlog met epics en/of user stories. De beschrijving bevat in ieder geval eisen voor (ondersteuning van) beheerfuncties die door de beoogd beheerder gesteld worden en voor logging, inclusief de (globale) inhoud van te loggen business events (gebeurtenissen op procesniveau) en de daarvoor geldende bewaartermijnen;
-- De ontwerp- en architectuurdocumentatie bestaat uit een projectstartarchitectuur (PSA), een softwarearchitectuurdocument (SAD), een infrastructuurarchitectuur (IA), een globaal functioneel ontwerp (GFO) bijvoorbeeld in de vorm van use cases, en een prototype en/of interactieontwerp. De architectuurdocumenten moeten expliciet inzichtelijk maken hoe aan de niet-functionele eisen wordt voldaan door uit te werken welke oplossingen en mechanieken gekozen zijn, bijvoorbeeld voor identificatie, authenticatie, autorisatie, concurrency, transactionele verwerking of logging;
-- De testdocumentatie bestaat uit een mastertestplan, gemaakt op basis van een productrisicoanalyse (PRA). Beveiligingstesten zijn een integraal onderdeel van het mastertestplan en worden als zodanig afgestemd met de opdrachtgever;
-- Het informatiebeveiligingsplan is gebaseerd op een dreigingen- en kwetsbaarhedenanalyse (TVA, threat and vulnerability assessment) en bevat een maatregelenselectie informatiebeveiliging. De TVA wordt tijdens de voorfase opgesteld op basis van de resultaten van de BIA, de eventuele PIA en inhoud van de ontwerp- en architectuurdocumentatie. Een TVA levert een deel van een traceerbare onderbouwing voor de te treffen beveiligingsmaatregelen;
+- De ontwerp- en architectuurdocumentatie bestaat uit een PSA (Projectstartarchitectuur), een SAD (Softwarearchitectuurdocument), een IA (Infrastructuurarchitectuur), een GFO (Globaal functioneel ontwerp) bijvoorbeeld in de vorm van use cases, en een prototype en/of interactieontwerp. De architectuurdocumenten moeten expliciet inzichtelijk maken hoe aan de niet-functionele eisen wordt voldaan door uit te werken welke oplossingen en mechanieken gekozen zijn, bijvoorbeeld voor identificatie, authenticatie, autorisatie, concurrency, transactionele verwerking of logging;
+- De testdocumentatie bestaat uit een mastertestplan, gemaakt op basis van een PRA (Productrisicoanalyse). Beveiligingstesten zijn een integraal onderdeel van het mastertestplan en worden als zodanig afgestemd met de opdrachtgever;
+- Het informatiebeveiligingsplan is gebaseerd op een dreigingen- en kwetsbaarhedenanalyse (TVA (Threat and vulnerability assessment)) en bevat een maatregelenselectie informatiebeveiliging. De TVA wordt tijdens de voorfase opgesteld op basis van de resultaten van de BIA, de eventuele PIA en inhoud van de ontwerp- en architectuurdocumentatie. Een TVA levert een deel van een traceerbare onderbouwing voor de te treffen beveiligingsmaatregelen;
 - Het vrijgaveadvies bevat ten minste alle nog openstaande testbevindingen en geconstateerde beveiligingsbevindingen. Zie ook [M26: Periodieke beoordeling informatiebeveiliging](#periodieke-beoordeling-informatiebeveiliging-m26-) en [M16: Verplichte tools](#verplichte-tools-m16-). Indien er beveiligingsissues zijn, zijn deze voorzien van een beschreven voorziene impact.
 - De deploymentdocumentatie bevat informatie over de eisen die een applicatie stelt aan een omgeving en de stappen die nodig zijn om de applicatie in die omgeving veilig te installeren en configureren. De documentatie bevat daartoe onder meer aanwijzingen voor de HTTP-header en -request-configuratie van de webserver en voor het verwijderen van overbodige header-informatie zoals de 'Server'-header. Ook zijn er aanwijzingen voor veilige configuratie(s) van (externe) toegang tot de beheerinterface. De documentatie bevat daarnaast in ieder geval een beschrijving van de protocollen en services die de applicatie aanbiedt, de protocollen, services en accounts die het product gebruikt en de protocollen, services en accounts die de applicatie gebruikt voor beheer;
 Zie de bijlage [Documenten voor M01: Op te leveren producten](#documenten-voor-m01-op-te-leveren-producten) voor een uitgebreider overzicht van de documenten en documentstandaarden die ICTU hanteert voor softwarerealisatieprojecten.
@@ -99,7 +99,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Gebruik van ISO-25010 (M13)
-De standaard ISO/IEC 25010:2011, kortweg "ISO-25010", biedt een model voor het beschrijven van productkwaliteit. Kwaliteitseigenschappen zijn voorzien van een naam, definitie en classificatie. ISO-25010 dekt een breed spectrum van kwaliteitseigenschappen af.
+De standaard ISO/IEC (International Electrotechnical Commission) 25010:2011, kortweg "ISO-25010", biedt een model voor het beschrijven van productkwaliteit. Kwaliteitseigenschappen zijn voorzien van een naam, definitie en classificatie. ISO-25010 dekt een breed spectrum van kwaliteitseigenschappen af.
 Voor specificatie en documentatie van vereiste en gewenste kwaliteitseigenschappen, de niet-functionele eisen, maken projecten gebruik van de terminologie uit ISO-25010. Projecten gebruiken ISO-25010 om te controleren of alle relevante kwaliteitseigenschappen van het op te leveren eindproduct worden meegenomen in de ontwikkeling en/of onderhoud van het product.
 Rationale
 De standaard ISO-25010 biedt een model voor productkwaliteit. De standaard biedt geen concrete maatregelen, maar biedt wel een begrippenkader en dekt het volledige spectrum van mogelijk relevante kwaliteitseigenschappen af. Het gebruiken van een standaard voor specificatie van kwaliteit voorkomt miscommunicatie over kwaliteitseigenschappen en de breedte van de standaard zorgt ervoor dat alle relevante aspecten aan bod komen.
@@ -124,7 +124,7 @@
 Rationale
 Het zo snel mogelijk en continu voldoen aan de kwaliteitsnormen beperkt toekomstige hersteltijd. Het dwingt tevens een structurele kwaliteitscontrole af.
 ICTU
-Bij ICTU wordt tijdens de voorfase van softwarerealisatieprojecten (zie ook [M14: Projecten splitsen in een voorbereidingsfase en een realisatiefase](#projecten-splitsen-in-een-voorbereidingsfase-en-een-realisatiefase-m14-)) het voldoen aan de kwaliteitsnormen met behulp van reviews gecontroleerd. Tijdens de realisatiefase van softwarerealisatieprojecten wordt het voldoen aan de kwaliteitsnormen diverse malen per uur gemeten door het 'Kwaliteitssysteem' (HQ). Het project kijkt dagelijks of er afwijkingen van de normen zijn en onderneemt actie indien nodig. Ook de kwaliteitsmanager signaleert afwijkingen en meldt deze bij het project. De ICTU-specifieke invulling van de kwaliteitsnormen is te vinden in het helpmenu van de geautomatiseerde kwaliteitsrapportages van ICTU.
+Bij ICTU wordt tijdens de voorfase van softwarerealisatieprojecten (zie ook [M14: Projecten splitsen in een voorbereidingsfase en een realisatiefase](#projecten-splitsen-in-een-voorbereidingsfase-en-een-realisatiefase-m14-)) het voldoen aan de kwaliteitsnormen met behulp van reviews gecontroleerd. Tijdens de realisatiefase van softwarerealisatieprojecten wordt het voldoen aan de kwaliteitsnormen diverse malen per uur gemeten door het 'Kwaliteitssysteem', genaamd HQ (Holistic Software Quality Reporting). Het project kijkt dagelijks of er afwijkingen van de normen zijn en onderneemt actie indien nodig. Ook de kwaliteitsmanager signaleert afwijkingen en meldt deze bij het project. De ICTU-specifieke invulling van de kwaliteitsnormen is te vinden in het helpmenu van de geautomatiseerde kwaliteitsrapportages van ICTU.
 </t>
         </r>
       </text>
@@ -178,12 +178,12 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Periodieke beoordeling informatiebeveiliging (M26)
-Projecten laten periodiek de beveiliging van de ontwikkelde software beoordelen. De code wordt zowel geautomatiseerd als handmatig door een beveiligingsexpert onderzocht op veelvoorkomende kwetsbaarheden en op het voldoen aan voorgeschreven normen. Overheidsspecifieke beveiligingsnormen of -raamwerken, zoals de Baseline Informatiebeveiliging Rijksdienst (BIR), bieden een basis voor de beoordeling.
+Projecten laten periodiek de beveiliging van de ontwikkelde software beoordelen. De code wordt zowel geautomatiseerd als handmatig door een beveiligingsexpert onderzocht op veelvoorkomende kwetsbaarheden en op het voldoen aan voorgeschreven normen. Overheidsspecifieke beveiligingsnormen of -raamwerken, zoals de BIR (Baseline Informatiebeveiliging Rijksdienst), bieden een basis voor de beoordeling.
 De projectorganisatie zorgt ervoor dat deze expertise op afroep beschikbaar gesteld kan worden aan projecten. Bevindingen uit de beveiligingstest worden vastgelegd als onderdeel van de werkvoorraad voor het ontwikkelproces (zie [M05: Iteratief en incrementeel ontwikkelproces](#iteratief-en-incrementeel-ontwikkelproces-m05-)).
 Rationale
 Door het inschakelen van actuele, specifieke expertise wordt de kans vergroot dat eventuele kwetsbaarheden in de gerealiseerde software tijdig herkend worden.
 ICTU
-Software wordt minimaal bij iedere grote release of ten minste twee keer per jaar onderworpen aan een beveiligingstest door beveiligingsexperts die ICTU daarvoor inhuurt. Op basis van documentatie en architectuurstudie, crystalbox security audits (broncodescan) en penetratieaudits beoordelen deze experts of de software voldoet aan de projectspecifieke niet-functionele eisen met betrekking tot beveiliging, of bekende kwetsbaarheden (OWASP) vermeden zijn en in hoeverre voldoende invulling gegeven is aan de normen vanuit die vanuit BIR en SSD gelden.
+Software wordt minimaal bij iedere grote release of ten minste twee keer per jaar onderworpen aan een beveiligingstest door beveiligingsexperts die ICTU daarvoor inhuurt. Op basis van documentatie en architectuurstudie, crystalbox security audits (broncodescan) en penetratieaudits beoordelen deze experts of de software voldoet aan de projectspecifieke niet-functionele eisen met betrekking tot beveiliging, of bekende kwetsbaarheden (zoals bijvoorbeeld in de OWASP Top 10 genoemd) vermeden zijn en in hoeverre voldoende invulling gegeven is aan de normen vanuit die vanuit BIR en SSD gelden.
 Indien door de opdrachtgever gewenst kunnen securitytesten door een onafhankelijke derde partij worden uitgevoerd in een daarvoor door de opdrachtgever beschikbaar gestelde omgeving. Dit kan zowel incidenteel als structureel worden ingericht. Afspraken hierover worden bij voorkeur al in de voorbereidingsfase gemaakt.
 De beveiligingstesten vinden plaats in aanvulling op de door tools uitgevoerde continue beveiligingsanalyse van de gerealiseerde software, zie [M16: Verplichte tools](#verplichte-tools-m16-). Bevindingen uit zowel een beveiligingstest als de continue analyse worden in Jira als issue - gemarkeerd als beveiligingsbugreport - vastgelegd op de backlog van het project.
 </t>
@@ -257,7 +257,7 @@
 Rationale
 Software incrementeel opleveren (zie [M05: Iteratief en incrementeel ontwikkelproces](#iteratief-en-incrementeel-ontwikkelproces-m05-)) vereist dat de software frequent gebouwd, getest en opgeleverd kan worden. Om dit efficiënt en foutvrij te doen, dient het proces van bouwen, testen en opleveren geautomatiseerd te zijn; een continuous delivery pipeline faciliteert dit.
 ICTU
-ICTU gebruikt Jenkins of Team Foundation Server (TFS) als tool voor de implementatie van de continuous delivery pipeline. De ICTU Release Manager ondersteunt de laatste stap (oplevering van het totale product).
+ICTU gebruikt Jenkins of TFS (Team Foundation Server) als tool voor de implementatie van de continuous delivery pipeline. De ICTU Release Manager ondersteunt de laatste stap (oplevering van het totale product).
 </t>
         </r>
       </text>
@@ -276,7 +276,7 @@
 Rationale
 De aanwezigheid van technische schuld heeft nadelige invloed op de kwaliteit van de eindproducten. Anderzijds is het ontstaan van technische schuld gedurende een project vaak onvermijdelijk. Het is daarnaast ook mogelijk dat een deel van de technische schuld bij aanvang van het project al bestond en mogelijk niet wordt opgelost. In alle gevallen is het verstandig om te weten welke technische schuld bestaat. Om te voorkomen dat technische schuld niet wordt opgelost en uitsluitend toeneemt, is het zaak om het verminderen van technische schuld planmatig aan te pakken.
 ICTU
-ICTU gebruikt [HQ](https://github.com/ICTU/quality-report/) (een door ICTU ontwikkeld, open source, geautomatiseerd kwaliteitssysteem) om bestaande technische schuld inzichtelijk te maken en de planning van het aflossen van de schuld vast te leggen, voor zover het technische schuld betreft van kwaliteitseigenschappen die HQ kan meten.
+ICTU gebruikt HQ (Holistic Software Quality Reporting), een door ICTU ontwikkeld, open source, geautomatiseerd kwaliteitssysteem, om bestaande technische schuld inzichtelijk te maken en de planning van het aflossen van de schuld vast te leggen, voor zover het technische schuld betreft van kwaliteitseigenschappen die HQ kan meten.
 </t>
         </r>
       </text>
@@ -483,7 +483,7 @@
           <t xml:space="preserve">Open source tools (M15)
 Bij de selectie van tools ter ondersteuning van de projectuitvoering  geeft de projectenorganisatie voorkeur aan open source tools.
 Rationale
-Conform de rationale uit NORA voor het gebruik van open source tools, zoals beschreven in NORA v3.0 drijfveer “beleid open standaarden” ([http://www.noraonline.nl/wiki/Beleid_open_standaarden](http://www.noraonline.nl/wiki/Beleid_open_standaarden)).
+Conform de rationale uit NORA (Nederlandse Overheid Referentiearchitectuur) voor het gebruik van open source tools, zoals beschreven in NORA v3.0 drijfveer “beleid open standaarden” ([http://www.noraonline.nl/wiki/Beleid_open_standaarden](http://www.noraonline.nl/wiki/Beleid_open_standaarden)).
 ICTU
 Tools die ICTU ontwikkelt ter ondersteuning van softwarerealisatieprojecten, worden bij voorkeur als open source beschikbaar gesteld.
 </t>
@@ -515,12 +515,12 @@
 ICTU
 ICTU gebruikt hiervoor de volgende tools:
 1. Jira - De 'eisen' worden, conform Scrumterminologie, geregistreerd als epics en/of user stories, de werkvoorraad als backlog, de iteraties als sprints,
-2. Jenkins voor Javaprojecten en Team Foundation Server (TFS) voor DotNet-projecten,
+2. Jenkins voor Javaprojecten en TFS (Team Foundation Server) voor DotNet-projecten,
 3. SonarQube,
 4. Release Manager,
-5. Reporting (Birt),
+5. Reporting (ontwikkeld met behulp van BIRT (Business Intelligence Reporting Tool)),
 6. Kwaliteitssysteem (HQ),
-7. OpenVAS en OWASP ZAP,
+7. OpenVAS (Vulnerability Assessment System) en OWASP (Open Web Application Security Project) ZAP (Zed Attack Proxy),
 8. OWASP Dependency Checker,
 9. Checkmarx.
 </t>
@@ -586,7 +586,7 @@
 Rationale
 Door het bieden van een afgeschermde digitale omgeving zijn de afhankelijkheden en invloeden tussen projecten minimaal en worden beveiligingsrisico's verkleind.
 ICTU
-ICTU ondersteunt dit met Docker en/of virtuele machines (VM) en een VLAN per project. Een nieuwe afgeschermde digitale omgeving is binnen een werkweek na aanvraag beschikbaar.
+ICTU ondersteunt dit met Docker en/of virtuele machines en een VLAN (Virtual local area network) per project. Een nieuwe afgeschermde digitale omgeving is binnen een werkweek na aanvraag beschikbaar.
 </t>
         </r>
       </text>
@@ -651,7 +651,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.2.1-build.4, 29-08-2018.</t>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.2.1-build.37, 31-08-2018.</t>
   </si>
   <si>
     <t>Maatregel</t>
@@ -675,10 +675,10 @@
     <t>Op te leveren producten</t>
   </si>
   <si>
-    <t>1. Business impact analysis (BIA)*</t>
-  </si>
-  <si>
-    <t>2. Privacy impact analysis (PIA)**</t>
+    <t>1. BIA (Business impact analysis)*</t>
+  </si>
+  <si>
+    <t>2. PIA (Privacy impact analysis)**</t>
   </si>
   <si>
     <t>3. Beschrijving van functionele eisen</t>
@@ -891,7 +891,7 @@
     <t>1. Een tool dat agile werken ondersteunt Bij ICTU: Jira - De 'eisen' worden, conform Scrumterminologie, geregistreerd als epics en/of user stories, de werkvoorraad als backlog, de iteraties als sprints,</t>
   </si>
   <si>
-    <t>2. Een tool dat het inrichten en uitvoeren van een continuous delivery pipeline ondersteunt. Bij ICTU: Jenkins voor Javaprojecten en Team Foundation Server (TFS) voor DotNet-projecten,</t>
+    <t>2. Een tool dat het inrichten en uitvoeren van een continuous delivery pipeline ondersteunt. Bij ICTU: Jenkins voor Javaprojecten en TFS (Team Foundation Server) voor DotNet-projecten,</t>
   </si>
   <si>
     <t>3. Een tool dat het monitoren van de kwaliteit van broncode ondersteunt. Bij ICTU: SonarQube,</t>
@@ -900,13 +900,13 @@
     <t>4. Een tool dat het releasen van software ondersteunt. Bij ICTU: Release Manager,</t>
   </si>
   <si>
-    <t>5. Een tool dat het maken van testrapportages ondersteunt. Bij ICTU: Reporting (Birt),</t>
+    <t>5. Een tool dat het maken van testrapportages ondersteunt. Bij ICTU: Reporting (ontwikkeld met behulp van BIRT (Business Intelligence Reporting Tool)),</t>
   </si>
   <si>
     <t>6. Een tool dat het maken van kwaliteitsrapportages ondersteunt. Bij ICTU: Kwaliteitssysteem (HQ),</t>
   </si>
   <si>
-    <t>7. Een tool dat de configuratie van de applicatie en de omgeving, waarbinnen die applicatie draait, controleert op bekende en veelvoorkomende kwetsbaarheden. Bij ICTU: OpenVAS en OWASP ZAP,</t>
+    <t>7. Een tool dat de configuratie van de applicatie en de omgeving, waarbinnen die applicatie draait, controleert op bekende en veelvoorkomende kwetsbaarheden. Bij ICTU: OpenVAS (Vulnerability Assessment System) en OWASP (Open Web Application Security Project) ZAP (Zed Attack Proxy),</t>
   </si>
   <si>
     <t>8. Een tool dat de door de applicatie gebruikte versies van externe bibliotheken, raamwerken of andersoortige bouwblokken scant op bekende kwetsbaarheden. Bij ICTU: OWASP Dependency Checker,</t>

</xml_diff>

<commit_message>
Generate appendix with abbreviations. (#94)
</commit_message>
<xml_diff>
--- a/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -44,10 +44,10 @@
           <t xml:space="preserve">Op te leveren producten (M01)
 Projecten zijn gesplitst in een voorbereidingsfase en een realisatiefase (zie [M14: Projecten splitsen in een voorbereidingsfase en een realisatiefase](#projecten-splitsen-in-een-voorbereidingsfase-en-een-realisatiefase-m14-)); alle fasen kennen specifieke producten. De onderstaande tabel benoemt de producten die een project in die fasen moet realiseren of waarover het project moet kunnen beschikken, indien er andere auteurs zijn (bijvoorbeeld de opdrachtgever). Het project zorgt voor een volledige oplevering van alle genoemde producten, waaronder de producten die niet door het project zelf zijn gemaakt.
 Als tijdens een project bestaande software dient te worden afgebouwd, onderhouden en/of herbouwd, vindt een onderzoek plaats naar de compleetheid en consistentie van de bestaande softwareproducten aan de hand van de onderstaande tabel (inclusief de deliverables in de kolom 'Realisatiefase') en wordt de kwaliteit van de bestaande software-producten getoetst ([M02: Continu voldoen aan kwaliteitsnormen](#continu-voldoen-aan-kwaliteitsnormen-m02-)). Dit onderzoek is onderdeel van de voorbereidingsfase en wordt uitgevoerd door vertegenwoordigers van de projectenorganisatie en medewerkers van het desbetreffende project.
-| Product                 | Voorbereidings᠆fase  | Voorbereidings᠆fase met onderzoek  | Realisatie᠆fase |
+| Product                | Voorbereidings᠆fase  | Voorbereidings᠆fase met onderzoek  | Realisatie᠆fase |
 |----------------------------------------------------------------------------------------|---|---|---|
-| Business impact analysis (BIA)*                                                        | ✔ | ✔ | ✔ |
-| Privacy impact analysis (PIA)**                                                        | ✔ | ✔ | ✔ |
+| BIA (Business impact analysis)*                                                        | ✔ | ✔ | ✔ |
+| PIA (Privacy impact analysis)**                                                        | ✔ | ✔ | ✔ |
 | Beschrijving van functionele eisen                                                     | ✔ | ✔ | ✔ |
 | Beschrijving van niet-functionele eisen                                                | ✔ | ✔ | ✔ |
 | Ontwerp- en architectuurdocumentatie (software, interactie, infrastructuur)            | ✔ | ✔ | ✔ |
@@ -76,11 +76,11 @@
 In een PIA legt de vragende organisatie vast wat de privacy-gevoeligheid is van de gegevens die in een proces of systeem worden verzameld en verwerkt. Zicht op privacygevoelige gegevens en het (laten) treffen van adequate en afdoende beschermingsmaatregelen is een wettelijke plicht die een organisatie niet aan een andere partij kan verdragen.
 ICTU
 ICTU hanteert de volgende documenten, templates en documentstandaarden voor softwarerealisatieprojecten:
-- De beschrijving van niet-functionele eisen is gebaseerd op ISO-25010, BIR en SSD, en bevat een prioritering van de niet-functionele eisen. De beschrijving van niet-functionele eisen is gebaseerd op het ICTU NFE-template. De beschrijving bevat in ieder geval eisen aan toegangsbeveiliging, aan beheerfuncties, aan logging en aan het gewenste gedrag van de software bij uitval van infrastructurele diensten, zoals een log-server;
+- De beschrijving van niet-functionele eisen is gebaseerd op ISO (International Organization for Standardization)-25010, de BIR (Baseline Informatiebeveiliging Rijksdienst) en de methode Grip op SSD (Secure software development) van het CIP (Centrum Informatiebeveiliging en Privacybescherming), en bevat een prioritering van de niet-functionele eisen. De beschrijving van niet-functionele eisen is gebaseerd op het ICTU NFE (Niet-functionele eisen)-template. De beschrijving bevat in ieder geval eisen aan toegangsbeveiliging, aan beheerfuncties, aan logging en aan het gewenste gedrag van de software bij uitval van infrastructurele diensten, zoals een log-server;
 - De beschrijving van functionele eisen bestaat uit een geprioriteerde backlog met epics en/of user stories. De beschrijving bevat in ieder geval eisen voor (ondersteuning van) beheerfuncties die door de beoogd beheerder gesteld worden en voor logging, inclusief de (globale) inhoud van te loggen business events (gebeurtenissen op procesniveau) en de daarvoor geldende bewaartermijnen;
-- De ontwerp- en architectuurdocumentatie bestaat uit een projectstartarchitectuur (PSA), een softwarearchitectuurdocument (SAD), een infrastructuurarchitectuur (IA), een globaal functioneel ontwerp (GFO) bijvoorbeeld in de vorm van use cases, en een prototype en/of interactieontwerp. De architectuurdocumenten moeten expliciet inzichtelijk maken hoe aan de niet-functionele eisen wordt voldaan door uit te werken welke oplossingen en mechanieken gekozen zijn, bijvoorbeeld voor identificatie, authenticatie, autorisatie, concurrency, transactionele verwerking of logging;
-- De testdocumentatie bestaat uit een mastertestplan, gemaakt op basis van een productrisicoanalyse (PRA). Beveiligingstesten zijn een integraal onderdeel van het mastertestplan en worden als zodanig afgestemd met de opdrachtgever;
-- Het informatiebeveiligingsplan is gebaseerd op een dreigingen- en kwetsbaarhedenanalyse (TVA, threat and vulnerability assessment) en bevat een maatregelenselectie informatiebeveiliging. De TVA wordt tijdens de voorfase opgesteld op basis van de resultaten van de BIA, de eventuele PIA en inhoud van de ontwerp- en architectuurdocumentatie. Een TVA levert een deel van een traceerbare onderbouwing voor de te treffen beveiligingsmaatregelen;
+- De ontwerp- en architectuurdocumentatie bestaat uit een PSA (Projectstartarchitectuur), een SAD (Softwarearchitectuurdocument), een IA (Infrastructuurarchitectuur), een GFO (Globaal functioneel ontwerp) bijvoorbeeld in de vorm van use cases, en een prototype en/of interactieontwerp. De architectuurdocumenten moeten expliciet inzichtelijk maken hoe aan de niet-functionele eisen wordt voldaan door uit te werken welke oplossingen en mechanieken gekozen zijn, bijvoorbeeld voor identificatie, authenticatie, autorisatie, concurrency, transactionele verwerking of logging;
+- De testdocumentatie bestaat uit een mastertestplan, gemaakt op basis van een PRA (Productrisicoanalyse). Beveiligingstesten zijn een integraal onderdeel van het mastertestplan en worden als zodanig afgestemd met de opdrachtgever;
+- Het informatiebeveiligingsplan is gebaseerd op een dreigingen- en kwetsbaarhedenanalyse (TVA (Threat and vulnerability assessment)) en bevat een maatregelenselectie informatiebeveiliging. De TVA wordt tijdens de voorfase opgesteld op basis van de resultaten van de BIA, de eventuele PIA en inhoud van de ontwerp- en architectuurdocumentatie. Een TVA levert een deel van een traceerbare onderbouwing voor de te treffen beveiligingsmaatregelen;
 - Het vrijgaveadvies bevat ten minste alle nog openstaande testbevindingen en geconstateerde beveiligingsbevindingen. Zie ook [M26: Periodieke beoordeling informatiebeveiliging](#periodieke-beoordeling-informatiebeveiliging-m26-) en [M16: Verplichte tools](#verplichte-tools-m16-). Indien er beveiligingsissues zijn, zijn deze voorzien van een beschreven voorziene impact.
 - De deploymentdocumentatie bevat informatie over de eisen die een applicatie stelt aan een omgeving en de stappen die nodig zijn om de applicatie in die omgeving veilig te installeren en configureren. De documentatie bevat daartoe onder meer aanwijzingen voor de HTTP-header en -request-configuratie van de webserver en voor het verwijderen van overbodige header-informatie zoals de 'Server'-header. Ook zijn er aanwijzingen voor veilige configuratie(s) van (externe) toegang tot de beheerinterface. De documentatie bevat daarnaast in ieder geval een beschrijving van de protocollen en services die de applicatie aanbiedt, de protocollen, services en accounts die het product gebruikt en de protocollen, services en accounts die de applicatie gebruikt voor beheer;
 Zie de bijlage [Documenten voor M01: Op te leveren producten](#documenten-voor-m01-op-te-leveren-producten) voor een uitgebreider overzicht van de documenten en documentstandaarden die ICTU hanteert voor softwarerealisatieprojecten.
@@ -99,7 +99,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Gebruik van ISO-25010 (M13)
-De standaard ISO/IEC 25010:2011, kortweg "ISO-25010", biedt een model voor het beschrijven van productkwaliteit. Kwaliteitseigenschappen zijn voorzien van een naam, definitie en classificatie. ISO-25010 dekt een breed spectrum van kwaliteitseigenschappen af.
+De standaard ISO/IEC (International Electrotechnical Commission) 25010:2011, kortweg "ISO-25010", biedt een model voor het beschrijven van productkwaliteit. Kwaliteitseigenschappen zijn voorzien van een naam, definitie en classificatie. ISO-25010 dekt een breed spectrum van kwaliteitseigenschappen af.
 Voor specificatie en documentatie van vereiste en gewenste kwaliteitseigenschappen, de niet-functionele eisen, maken projecten gebruik van de terminologie uit ISO-25010. Projecten gebruiken ISO-25010 om te controleren of alle relevante kwaliteitseigenschappen van het op te leveren eindproduct worden meegenomen in de ontwikkeling en/of onderhoud van het product.
 Rationale
 De standaard ISO-25010 biedt een model voor productkwaliteit. De standaard biedt geen concrete maatregelen, maar biedt wel een begrippenkader en dekt het volledige spectrum van mogelijk relevante kwaliteitseigenschappen af. Het gebruiken van een standaard voor specificatie van kwaliteit voorkomt miscommunicatie over kwaliteitseigenschappen en de breedte van de standaard zorgt ervoor dat alle relevante aspecten aan bod komen.
@@ -124,7 +124,7 @@
 Rationale
 Het zo snel mogelijk en continu voldoen aan de kwaliteitsnormen beperkt toekomstige hersteltijd. Het dwingt tevens een structurele kwaliteitscontrole af.
 ICTU
-Bij ICTU wordt tijdens de voorfase van softwarerealisatieprojecten (zie ook [M14: Projecten splitsen in een voorbereidingsfase en een realisatiefase](#projecten-splitsen-in-een-voorbereidingsfase-en-een-realisatiefase-m14-)) het voldoen aan de kwaliteitsnormen met behulp van reviews gecontroleerd. Tijdens de realisatiefase van softwarerealisatieprojecten wordt het voldoen aan de kwaliteitsnormen diverse malen per uur gemeten door het 'Kwaliteitssysteem' (HQ). Het project kijkt dagelijks of er afwijkingen van de normen zijn en onderneemt actie indien nodig. Ook de kwaliteitsmanager signaleert afwijkingen en meldt deze bij het project. De ICTU-specifieke invulling van de kwaliteitsnormen is te vinden in het helpmenu van de geautomatiseerde kwaliteitsrapportages van ICTU.
+Bij ICTU wordt tijdens de voorfase van softwarerealisatieprojecten (zie ook [M14: Projecten splitsen in een voorbereidingsfase en een realisatiefase](#projecten-splitsen-in-een-voorbereidingsfase-en-een-realisatiefase-m14-)) het voldoen aan de kwaliteitsnormen met behulp van reviews gecontroleerd. Tijdens de realisatiefase van softwarerealisatieprojecten wordt het voldoen aan de kwaliteitsnormen diverse malen per uur gemeten door het 'Kwaliteitssysteem', genaamd HQ (Holistic Software Quality Reporting). Het project kijkt dagelijks of er afwijkingen van de normen zijn en onderneemt actie indien nodig. Ook de kwaliteitsmanager signaleert afwijkingen en meldt deze bij het project. De ICTU-specifieke invulling van de kwaliteitsnormen is te vinden in het helpmenu van de geautomatiseerde kwaliteitsrapportages van ICTU.
 </t>
         </r>
       </text>
@@ -178,12 +178,12 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Periodieke beoordeling informatiebeveiliging (M26)
-Projecten laten periodiek de beveiliging van de ontwikkelde software beoordelen. De code wordt zowel geautomatiseerd als handmatig door een beveiligingsexpert onderzocht op veelvoorkomende kwetsbaarheden en op het voldoen aan voorgeschreven normen. Overheidsspecifieke beveiligingsnormen of -raamwerken, zoals de Baseline Informatiebeveiliging Rijksdienst (BIR), bieden een basis voor de beoordeling.
+Projecten laten periodiek de beveiliging van de ontwikkelde software beoordelen. De code wordt zowel geautomatiseerd als handmatig door een beveiligingsexpert onderzocht op veelvoorkomende kwetsbaarheden en op het voldoen aan voorgeschreven normen. Overheidsspecifieke beveiligingsnormen of -raamwerken, zoals de BIR (Baseline Informatiebeveiliging Rijksdienst), bieden een basis voor de beoordeling.
 De projectorganisatie zorgt ervoor dat deze expertise op afroep beschikbaar gesteld kan worden aan projecten. Bevindingen uit de beveiligingstest worden vastgelegd als onderdeel van de werkvoorraad voor het ontwikkelproces (zie [M05: Iteratief en incrementeel ontwikkelproces](#iteratief-en-incrementeel-ontwikkelproces-m05-)).
 Rationale
 Door het inschakelen van actuele, specifieke expertise wordt de kans vergroot dat eventuele kwetsbaarheden in de gerealiseerde software tijdig herkend worden.
 ICTU
-Software wordt minimaal bij iedere grote release of ten minste twee keer per jaar onderworpen aan een beveiligingstest door beveiligingsexperts die ICTU daarvoor inhuurt. Op basis van documentatie en architectuurstudie, crystalbox security audits (broncodescan) en penetratieaudits beoordelen deze experts of de software voldoet aan de projectspecifieke niet-functionele eisen met betrekking tot beveiliging, of bekende kwetsbaarheden (OWASP) vermeden zijn en in hoeverre voldoende invulling gegeven is aan de normen vanuit die vanuit BIR en SSD gelden.
+Software wordt minimaal bij iedere grote release of ten minste twee keer per jaar onderworpen aan een beveiligingstest door beveiligingsexperts die ICTU daarvoor inhuurt. Op basis van documentatie en architectuurstudie, crystalbox security audits (broncodescan) en penetratieaudits beoordelen deze experts of de software voldoet aan de projectspecifieke niet-functionele eisen met betrekking tot beveiliging, of bekende kwetsbaarheden (zoals bijvoorbeeld in de OWASP Top 10 genoemd) vermeden zijn en in hoeverre voldoende invulling gegeven is aan de normen vanuit die vanuit BIR en SSD gelden.
 Indien door de opdrachtgever gewenst kunnen securitytesten door een onafhankelijke derde partij worden uitgevoerd in een daarvoor door de opdrachtgever beschikbaar gestelde omgeving. Dit kan zowel incidenteel als structureel worden ingericht. Afspraken hierover worden bij voorkeur al in de voorbereidingsfase gemaakt.
 De beveiligingstesten vinden plaats in aanvulling op de door tools uitgevoerde continue beveiligingsanalyse van de gerealiseerde software, zie [M16: Verplichte tools](#verplichte-tools-m16-). Bevindingen uit zowel een beveiligingstest als de continue analyse worden in Jira als issue - gemarkeerd als beveiligingsbugreport - vastgelegd op de backlog van het project.
 </t>
@@ -257,7 +257,7 @@
 Rationale
 Software incrementeel opleveren (zie [M05: Iteratief en incrementeel ontwikkelproces](#iteratief-en-incrementeel-ontwikkelproces-m05-)) vereist dat de software frequent gebouwd, getest en opgeleverd kan worden. Om dit efficiënt en foutvrij te doen, dient het proces van bouwen, testen en opleveren geautomatiseerd te zijn; een continuous delivery pipeline faciliteert dit.
 ICTU
-ICTU gebruikt Jenkins of Team Foundation Server (TFS) als tool voor de implementatie van de continuous delivery pipeline. De ICTU Release Manager ondersteunt de laatste stap (oplevering van het totale product).
+ICTU gebruikt Jenkins of TFS (Team Foundation Server) als tool voor de implementatie van de continuous delivery pipeline. De ICTU Release Manager ondersteunt de laatste stap (oplevering van het totale product).
 </t>
         </r>
       </text>
@@ -276,7 +276,7 @@
 Rationale
 De aanwezigheid van technische schuld heeft nadelige invloed op de kwaliteit van de eindproducten. Anderzijds is het ontstaan van technische schuld gedurende een project vaak onvermijdelijk. Het is daarnaast ook mogelijk dat een deel van de technische schuld bij aanvang van het project al bestond en mogelijk niet wordt opgelost. In alle gevallen is het verstandig om te weten welke technische schuld bestaat. Om te voorkomen dat technische schuld niet wordt opgelost en uitsluitend toeneemt, is het zaak om het verminderen van technische schuld planmatig aan te pakken.
 ICTU
-ICTU gebruikt [HQ](https://github.com/ICTU/quality-report/) (een door ICTU ontwikkeld, open source, geautomatiseerd kwaliteitssysteem) om bestaande technische schuld inzichtelijk te maken en de planning van het aflossen van de schuld vast te leggen, voor zover het technische schuld betreft van kwaliteitseigenschappen die HQ kan meten.
+ICTU gebruikt HQ (Holistic Software Quality Reporting), een door ICTU ontwikkeld, open source, geautomatiseerd kwaliteitssysteem, om bestaande technische schuld inzichtelijk te maken en de planning van het aflossen van de schuld vast te leggen, voor zover het technische schuld betreft van kwaliteitseigenschappen die HQ kan meten.
 </t>
         </r>
       </text>
@@ -483,7 +483,7 @@
           <t xml:space="preserve">Open source tools (M15)
 Bij de selectie van tools ter ondersteuning van de projectuitvoering  geeft de projectenorganisatie voorkeur aan open source tools.
 Rationale
-Conform de rationale uit NORA voor het gebruik van open source tools, zoals beschreven in NORA v3.0 drijfveer “beleid open standaarden” ([http://www.noraonline.nl/wiki/Beleid_open_standaarden](http://www.noraonline.nl/wiki/Beleid_open_standaarden)).
+Conform de rationale uit NORA (Nederlandse Overheid Referentiearchitectuur) voor het gebruik van open source tools, zoals beschreven in NORA v3.0 drijfveer “beleid open standaarden” ([http://www.noraonline.nl/wiki/Beleid_open_standaarden](http://www.noraonline.nl/wiki/Beleid_open_standaarden)).
 ICTU
 Tools die ICTU ontwikkelt ter ondersteuning van softwarerealisatieprojecten, worden bij voorkeur als open source beschikbaar gesteld.
 </t>
@@ -515,12 +515,12 @@
 ICTU
 ICTU gebruikt hiervoor de volgende tools:
 1. Jira - De 'eisen' worden, conform Scrumterminologie, geregistreerd als epics en/of user stories, de werkvoorraad als backlog, de iteraties als sprints,
-2. Jenkins voor Javaprojecten en Team Foundation Server (TFS) voor DotNet-projecten,
+2. Jenkins voor Javaprojecten en TFS (Team Foundation Server) voor DotNet-projecten,
 3. SonarQube,
 4. Release Manager,
-5. Reporting (Birt),
+5. Reporting (ontwikkeld met behulp van BIRT (Business Intelligence Reporting Tool)),
 6. Kwaliteitssysteem (HQ),
-7. OpenVAS en OWASP ZAP,
+7. OpenVAS (Vulnerability Assessment System) en OWASP (Open Web Application Security Project) ZAP (Zed Attack Proxy),
 8. OWASP Dependency Checker,
 9. Checkmarx.
 </t>
@@ -586,7 +586,7 @@
 Rationale
 Door het bieden van een afgeschermde digitale omgeving zijn de afhankelijkheden en invloeden tussen projecten minimaal en worden beveiligingsrisico's verkleind.
 ICTU
-ICTU ondersteunt dit met Docker en/of virtuele machines (VM) en een VLAN per project. Een nieuwe afgeschermde digitale omgeving is binnen een werkweek na aanvraag beschikbaar.
+ICTU ondersteunt dit met Docker en/of virtuele machines en een VLAN (Virtual local area network) per project. Een nieuwe afgeschermde digitale omgeving is binnen een werkweek na aanvraag beschikbaar.
 </t>
         </r>
       </text>
@@ -651,7 +651,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.2.1-build.4, 29-08-2018.</t>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.2.1-build.38, 31-08-2018.</t>
   </si>
   <si>
     <t>Maatregel</t>
@@ -675,10 +675,10 @@
     <t>Op te leveren producten</t>
   </si>
   <si>
-    <t>1. Business impact analysis (BIA)*</t>
-  </si>
-  <si>
-    <t>2. Privacy impact analysis (PIA)**</t>
+    <t>1. BIA (Business impact analysis)*</t>
+  </si>
+  <si>
+    <t>2. PIA (Privacy impact analysis)**</t>
   </si>
   <si>
     <t>3. Beschrijving van functionele eisen</t>
@@ -891,7 +891,7 @@
     <t>1. Een tool dat agile werken ondersteunt Bij ICTU: Jira - De 'eisen' worden, conform Scrumterminologie, geregistreerd als epics en/of user stories, de werkvoorraad als backlog, de iteraties als sprints,</t>
   </si>
   <si>
-    <t>2. Een tool dat het inrichten en uitvoeren van een continuous delivery pipeline ondersteunt. Bij ICTU: Jenkins voor Javaprojecten en Team Foundation Server (TFS) voor DotNet-projecten,</t>
+    <t>2. Een tool dat het inrichten en uitvoeren van een continuous delivery pipeline ondersteunt. Bij ICTU: Jenkins voor Javaprojecten en TFS (Team Foundation Server) voor DotNet-projecten,</t>
   </si>
   <si>
     <t>3. Een tool dat het monitoren van de kwaliteit van broncode ondersteunt. Bij ICTU: SonarQube,</t>
@@ -900,13 +900,13 @@
     <t>4. Een tool dat het releasen van software ondersteunt. Bij ICTU: Release Manager,</t>
   </si>
   <si>
-    <t>5. Een tool dat het maken van testrapportages ondersteunt. Bij ICTU: Reporting (Birt),</t>
+    <t>5. Een tool dat het maken van testrapportages ondersteunt. Bij ICTU: Reporting (ontwikkeld met behulp van BIRT (Business Intelligence Reporting Tool)),</t>
   </si>
   <si>
     <t>6. Een tool dat het maken van kwaliteitsrapportages ondersteunt. Bij ICTU: Kwaliteitssysteem (HQ),</t>
   </si>
   <si>
-    <t>7. Een tool dat de configuratie van de applicatie en de omgeving, waarbinnen die applicatie draait, controleert op bekende en veelvoorkomende kwetsbaarheden. Bij ICTU: OpenVAS en OWASP ZAP,</t>
+    <t>7. Een tool dat de configuratie van de applicatie en de omgeving, waarbinnen die applicatie draait, controleert op bekende en veelvoorkomende kwetsbaarheden. Bij ICTU: OpenVAS (Vulnerability Assessment System) en OWASP (Open Web Application Security Project) ZAP (Zed Attack Proxy),</t>
   </si>
   <si>
     <t>8. Een tool dat de door de applicatie gebruikte versies van externe bibliotheken, raamwerken of andersoortige bouwblokken scant op bekende kwetsbaarheden. Bij ICTU: OWASP Dependency Checker,</t>

</xml_diff>

<commit_message>
Update deelnemers M10: periodiek projectoverleg.
</commit_message>
<xml_diff>
--- a/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -319,7 +319,7 @@
           </rPr>
           <t xml:space="preserve">Periodiek projectoverleg (M10)
 De projectverantwoordelijke organiseert een periodiek projectoverleg. Dit overleg vindt wekelijks plaats en duurt niet langer dan een uur.
-Vereiste aanwezigen zijn de project-verantwoordelijke, een vertegenwoordiger uit het projectteam en een kwaliteitsmanager. Andere aanwezigen kunnen zijn: opdrachtnemer, architecten en coaches.
+Vereiste aanwezigen zijn de projectverantwoordelijke, een vertegenwoordiger uit elk van de realiserende teams en de kwaliteitsmanager van het project. Andere aanwezigen kunnen zijn: de projectarchitect en de product owner.
 De agenda voor dit overleg bestaat ten minste uit de volgende onderwerpen:
 - mededelingen - pro-actief informeren over voor het project relevante ontwikkelingen,
 - actie- en besluitenlijst,
@@ -328,7 +328,7 @@
 - kwaliteit en architectuur - bespreking van kwaliteit (bijvoorbeeld naar aanleiding van de self-assessment), architectuur (voor borging van inhoudelijke koers), eventuele afwijkingen en benodigde acties,
 - risico's en aandachtspunten.
 Rationale
-Het doel van het periodiek projectoverleg is alle directe betrokkenen, breder dan het realiserende team, op hetzelfde informatieniveau te brengen en te houden. Directe betrokkenen zijn alle medewerkers die geen onderdeel uitmaken van het realiserende team, maar wel verantwoordelijkheid dragen voor het projectsucces.
+Het doel van het periodiek projectoverleg is alle directe betrokkenen, breder dan de realiserende teams, op hetzelfde informatieniveau te brengen en te houden. Directe betrokkenen zijn alle medewerkers die geen onderdeel uitmaken van de realiserende teams, maar wel verantwoordelijkheid dragen voor het projectsucces.
 ICTU
 Bij periodiek projectoverleg zijn de software delivery manager, de kwaliteitsmanager en de Scrum master vereist.
 </t>
@@ -587,6 +587,7 @@
 Door het bieden van een afgeschermde digitale omgeving zijn de afhankelijkheden en invloeden tussen projecten minimaal en worden beveiligingsrisico's verkleind.
 ICTU
 ICTU ondersteunt dit met Docker en/of virtuele machines en een VLAN (Virtual local area network) per project. Een nieuwe afgeschermde digitale omgeving is binnen een werkweek na aanvraag beschikbaar.
+Bij ICTU beheert het team ITB (ISR technisch beheer) de basisconfiguratie van de afgeschermde digitale omgevingen. Projectteams wijken alleen in overleg met het ITB-team af van de basisconfiguratie. Als bepaalde afwijkingen vaker voorkomen, kan dit leiden tot het maken van aanpassingen aan de basisconfiguratie.
 </t>
         </r>
       </text>
@@ -651,7 +652,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.2.1-build.38, 31-08-2018.</t>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.2.1-build.41, 16-01-2019.</t>
   </si>
   <si>
     <t>Maatregel</t>

</xml_diff>

<commit_message>
Update deelnemers M10: periodiek projectoverleg. (#105)
</commit_message>
<xml_diff>
--- a/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -319,7 +319,7 @@
           </rPr>
           <t xml:space="preserve">Periodiek projectoverleg (M10)
 De projectverantwoordelijke organiseert een periodiek projectoverleg. Dit overleg vindt wekelijks plaats en duurt niet langer dan een uur.
-Vereiste aanwezigen zijn de project-verantwoordelijke, een vertegenwoordiger uit het projectteam en een kwaliteitsmanager. Andere aanwezigen kunnen zijn: opdrachtnemer, architecten en coaches.
+Vereiste aanwezigen zijn de projectverantwoordelijke, een vertegenwoordiger uit elk van de realiserende teams en de kwaliteitsmanager van het project. Andere aanwezigen kunnen zijn: de projectarchitect en de product owner.
 De agenda voor dit overleg bestaat ten minste uit de volgende onderwerpen:
 - mededelingen - pro-actief informeren over voor het project relevante ontwikkelingen,
 - actie- en besluitenlijst,
@@ -328,7 +328,7 @@
 - kwaliteit en architectuur - bespreking van kwaliteit (bijvoorbeeld naar aanleiding van de self-assessment), architectuur (voor borging van inhoudelijke koers), eventuele afwijkingen en benodigde acties,
 - risico's en aandachtspunten.
 Rationale
-Het doel van het periodiek projectoverleg is alle directe betrokkenen, breder dan het realiserende team, op hetzelfde informatieniveau te brengen en te houden. Directe betrokkenen zijn alle medewerkers die geen onderdeel uitmaken van het realiserende team, maar wel verantwoordelijkheid dragen voor het projectsucces.
+Het doel van het periodiek projectoverleg is alle directe betrokkenen, breder dan de realiserende teams, op hetzelfde informatieniveau te brengen en te houden. Directe betrokkenen zijn alle medewerkers die geen onderdeel uitmaken van de realiserende teams, maar wel verantwoordelijkheid dragen voor het projectsucces.
 ICTU
 Bij periodiek projectoverleg zijn de software delivery manager, de kwaliteitsmanager en de Scrum master vereist.
 </t>
@@ -587,6 +587,7 @@
 Door het bieden van een afgeschermde digitale omgeving zijn de afhankelijkheden en invloeden tussen projecten minimaal en worden beveiligingsrisico's verkleind.
 ICTU
 ICTU ondersteunt dit met Docker en/of virtuele machines en een VLAN (Virtual local area network) per project. Een nieuwe afgeschermde digitale omgeving is binnen een werkweek na aanvraag beschikbaar.
+Bij ICTU beheert het team ITB (ISR technisch beheer) de basisconfiguratie van de afgeschermde digitale omgevingen. Projectteams wijken alleen in overleg met het ITB-team af van de basisconfiguratie. Als bepaalde afwijkingen vaker voorkomen, kan dit leiden tot het maken van aanpassingen aan de basisconfiguratie.
 </t>
         </r>
       </text>
@@ -651,7 +652,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.2.1-build.38, 31-08-2018.</t>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.2.1-build.41, 16-01-2019.</t>
   </si>
   <si>
     <t>Maatregel</t>

</xml_diff>

<commit_message>
Add action list to self-assessment workbook.
</commit_message>
<xml_diff>
--- a/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Self-assessment checklist" sheetId="1" r:id="rId1"/>
+    <sheet name="Self-assessment verbeteracties" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -654,9 +655,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
-  <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.3.1-build.1, 01-05-2019.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="108">
+  <si>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 2.0-build.0, 14-08-2019.</t>
   </si>
   <si>
     <t>Maatregel</t>
@@ -969,6 +970,15 @@
   </si>
   <si>
     <t>Warme kennisoverdracht</t>
+  </si>
+  <si>
+    <t>Onderstaande actielijst kan gebruikt worden om acties n.a.v. de self-assessment bij te houden.</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Actie</t>
   </si>
 </sst>
 </file>
@@ -2102,4 +2112,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="70.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" ht="30" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add action list to self-assessment workbook. (#126)
* Add action list to self-assessment workbook.
</commit_message>
<xml_diff>
--- a/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Self-assessment checklist" sheetId="1" r:id="rId1"/>
+    <sheet name="Self-assessment verbeteracties" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -654,9 +655,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
-  <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.3.1-build.1, 01-05-2019.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="108">
+  <si>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 2.0-build.0, 14-08-2019.</t>
   </si>
   <si>
     <t>Maatregel</t>
@@ -969,6 +970,15 @@
   </si>
   <si>
     <t>Warme kennisoverdracht</t>
+  </si>
+  <si>
+    <t>Onderstaande actielijst kan gebruikt worden om acties n.a.v. de self-assessment bij te houden.</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Actie</t>
   </si>
 </sst>
 </file>
@@ -2102,4 +2112,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="70.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" ht="30" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
herformulering verplicht gebruik, toevoeging tool voor versiebeheer (#125)
Herformulering verplicht gebruik, toevoeging tool voor versiebeheer. Closes #117.
</commit_message>
<xml_diff>
--- a/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -504,35 +504,37 @@
             <family val="2"/>
           </rPr>
           <t>Verplichte tools (M16)
-De projectenorganisatie stelt het gebruik van de volgende tools voor alle projecten verplicht:
-1. Een tool dat agile werken ondersteunt. Een dergelijk tool voorziet in het opvoeren van eisen, het opvoeren van logische testgevallen en het koppelen van logische testgevallen aan eisen, het bijhouden van een werkvoorraad, het plannen van iteraties en het toewijzen van eisen aan iteraties.
-2. Een tool dat het inrichten en uitvoeren van een continuous delivery pipeline ondersteunt.
-3. Een tool dat het monitoren van de kwaliteit van broncode ondersteunt.
-4. Een tool dat het releasen van software ondersteunt.
-5. Een tool dat het maken van testrapportages ondersteunt.
-6. Een tool dat het maken van kwaliteitsrapportages ondersteunt.
-7. Een tool dat de configuratie van de applicatie en de omgeving, waarbinnen die applicatie draait, controleert op bekende en veelvoorkomende kwetsbaarheden.
-8. Een tool dat de door de applicatie gebruikte versies van externe bibliotheken, raamwerken of andersoortige bouwblokken scant op bekende kwetsbaarheden.
-9. Een tool dat de broncode geautomatiseerd beoordeelt op het voorkomen van bekende kwetsbare constructies.
-10. Een tool dat het testen van toegankelijkheid ondersteunt.
-Rationale
-Projecten hebben een redelijke vrijheid bij het kiezen van tools, maar het gebruik van een aantal is verplicht gesteld. Deze tools zijn nodig voor een efficiënte uitvoering van deze kwaliteitsaanpak. Uniform gebruik van deze tools maakt het mogelijk koppeling tussen die tools voor alle projecten te standaardiseren. Daarnaast bevordert het de uitwisselbaarheid van medewerkers en neemt het risico op het gebruik van onvolwassen tools af.
-ICTU
-ICTU gebruikt hiervoor de volgende tools:
+De projectenorganisatie stelt het gebruik van tools voor de volgende taken verplicht:
+1. agile werken, waaronder het opvoeren van eisen, het opvoeren van logische testgevallen, het koppelen van logische testgevallen aan eisen, het bijhouden van een werkvoorraad, het plannen van iteraties en het toewijzen van eisen aan iteraties,
+2. inrichten en uitvoeren van een continuous delivery pipeline,
+3. monitoren van de kwaliteit van broncode,
+4. versiebeheer van op te leveren producten, waaronder broncode, configuratiebestanden en documentatie,
+5. release van software,
+6. maken van testrapportages,
+7. maken van kwaliteitsrapportages,
+8. controleren van de configuratie van de applicatie en de omgeving, waarbinnen die applicatie draait, op aanwezigheid bekende kwetsbaarheden,
+9. controleren van door de applicatie gebruikte versies van externe bibliotheken, raamwerken of andersoortige bouwblokken op aanwezigheid bekende kwetsbaarheden,
+10. controleren van de broncode op aanwezigheid bekende kwetsbare constructies,
+11. testen op toegankelijkheid van de applicatie.
+Rationale
+Projecten hebben een redelijke vrijheid bij het kiezen en gebruiken van tools, maar voor een aantal taken is het gebruik verplicht gesteld. Deze tools zijn nodig voor een efficiënte uitvoering van de kwaliteitsaanpak. Uniform gebruik van deze tools maakt het mogelijk koppeling tussen die tools voor alle projecten te standaardiseren; daarnaast bevordert het de uitwisselbaarheid van medewerkers en neemt het risico op het gebruik van onvolwassen tools af. Tot slot is het gebruik in een aantal gevallen, ten behoeve van informatiebeveiliging bij de overheid, verplicht.
+ICTU
+ICTU ondersteunt hiervoor de volgende tools:
 1. Jira - De 'eisen' worden, conform Scrumterminologie, geregistreerd als epics en/of user stories, de werkvoorraad als backlog, de iteraties als sprints,
 2. Jenkins voor Javaprojecten en TFS (Team Foundation Server) voor DotNet-projecten,
 3. SonarQube,
-4. Release Manager,
-5. Reporting (ontwikkeld met behulp van BIRT (Business Intelligence Reporting Tool)),
-6. Kwaliteitssysteem (HQ),
-7. OpenVAS (Vulnerability Assessment System) en OWASP (Open Web Application Security Project) ZAP (Zed Attack Proxy),
-8. OWASP Dependency Checker,
-9. Checkmarx,
-10. Axe.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B68" authorId="0">
+4. GitLab en TFS,
+5. Release Manager,
+6. Reporting (ontwikkeld met behulp van Business Intelligence Reporting Tool, BIRT),
+7. HQ en Quality Time,
+8. OpenVAS (Vulnerability Assessment System) en OWASP (Open Web Application Security Project) ZAP (Zed Attack Proxy),
+9. OWASP Dependency Checker,
+10. Checkmarx,
+11. Axe.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B69" authorId="0">
       <text>
         <r>
           <rPr>
@@ -558,7 +560,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B72" authorId="0">
+    <comment ref="B73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -577,7 +579,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B73" authorId="0">
+    <comment ref="B74" authorId="0">
       <text>
         <r>
           <rPr>
@@ -597,7 +599,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B74" authorId="0">
+    <comment ref="B75" authorId="0">
       <text>
         <r>
           <rPr>
@@ -614,7 +616,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B75" authorId="0">
+    <comment ref="B76" authorId="0">
       <text>
         <r>
           <rPr>
@@ -633,7 +635,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B76" authorId="0">
+    <comment ref="B77" authorId="0">
       <text>
         <r>
           <rPr>
@@ -655,9 +657,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="108">
-  <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 2.0-build.0, 14-08-2019.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
+  <si>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de Kwaliteitsaanpak ICTU Software Realisatie versie 1.3.1-build.2, 14-08-2019.</t>
   </si>
   <si>
     <t>Maatregel</t>
@@ -897,34 +899,37 @@
     <t>Verplichte tools</t>
   </si>
   <si>
-    <t>1. Een tool dat agile werken ondersteunt Bij ICTU: Jira - De 'eisen' worden, conform Scrumterminologie, geregistreerd als epics en/of user stories, de werkvoorraad als backlog, de iteraties als sprints,</t>
-  </si>
-  <si>
-    <t>2. Een tool dat het inrichten en uitvoeren van een continuous delivery pipeline ondersteunt. Bij ICTU: Jenkins voor Javaprojecten en TFS (Team Foundation Server) voor DotNet-projecten,</t>
-  </si>
-  <si>
-    <t>3. Een tool dat het monitoren van de kwaliteit van broncode ondersteunt. Bij ICTU: SonarQube,</t>
-  </si>
-  <si>
-    <t>4. Een tool dat het releasen van software ondersteunt. Bij ICTU: Release Manager,</t>
-  </si>
-  <si>
-    <t>5. Een tool dat het maken van testrapportages ondersteunt. Bij ICTU: Reporting (ontwikkeld met behulp van BIRT (Business Intelligence Reporting Tool)),</t>
-  </si>
-  <si>
-    <t>6. Een tool dat het maken van kwaliteitsrapportages ondersteunt. Bij ICTU: Kwaliteitssysteem (HQ),</t>
-  </si>
-  <si>
-    <t>7. Een tool dat de configuratie van de applicatie en de omgeving, waarbinnen die applicatie draait, controleert op bekende en veelvoorkomende kwetsbaarheden. Bij ICTU: OpenVAS (Vulnerability Assessment System) en OWASP (Open Web Application Security Project) ZAP (Zed Attack Proxy),</t>
-  </si>
-  <si>
-    <t>8. Een tool dat de door de applicatie gebruikte versies van externe bibliotheken, raamwerken of andersoortige bouwblokken scant op bekende kwetsbaarheden. Bij ICTU: OWASP Dependency Checker,</t>
-  </si>
-  <si>
-    <t>9. Een tool dat de broncode geautomatiseerd beoordeelt op het voorkomen van bekende kwetsbare constructies. Bij ICTU: Checkmarx,</t>
-  </si>
-  <si>
-    <t>10. Een tool dat het testen van toegankelijkheid ondersteunt. Bij ICTU: Axe.</t>
+    <t>1. agile werken, waaronder het opvoeren van eisen, het opvoeren van logische testgevallen, het koppelen van logische testgevallen aan eisen, het bijhouden van een werkvoorraad, het plannen van iteraties en het toewijzen van eisen aan iteraties, Bij ICTU: Jira - De 'eisen' worden, conform Scrumterminologie, geregistreerd als epics en/of user stories, de werkvoorraad als backlog, de iteraties als sprints,</t>
+  </si>
+  <si>
+    <t>2. inrichten en uitvoeren van een continuous delivery pipeline, Bij ICTU: Jenkins voor Javaprojecten en TFS (Team Foundation Server) voor DotNet-projecten,</t>
+  </si>
+  <si>
+    <t>3. monitoren van de kwaliteit van broncode, Bij ICTU: SonarQube,</t>
+  </si>
+  <si>
+    <t>4. versiebeheer van op te leveren producten, waaronder broncode, configuratiebestanden en documentatie, Bij ICTU: GitLab en TFS,</t>
+  </si>
+  <si>
+    <t>5. release van software, Bij ICTU: Release Manager,</t>
+  </si>
+  <si>
+    <t>6. maken van testrapportages, Bij ICTU: Reporting (ontwikkeld met behulp van Business Intelligence Reporting Tool, BIRT),</t>
+  </si>
+  <si>
+    <t>7. maken van kwaliteitsrapportages, Bij ICTU: HQ en Quality Time,</t>
+  </si>
+  <si>
+    <t>8. controleren van de configuratie van de applicatie en de omgeving, waarbinnen die applicatie draait, op aanwezigheid bekende kwetsbaarheden, Bij ICTU: OpenVAS (Vulnerability Assessment System) en OWASP (Open Web Application Security Project) ZAP (Zed Attack Proxy),</t>
+  </si>
+  <si>
+    <t>9. controleren van door de applicatie gebruikte versies van externe bibliotheken, raamwerken of andersoortige bouwblokken op aanwezigheid bekende kwetsbaarheden, Bij ICTU: OWASP Dependency Checker,</t>
+  </si>
+  <si>
+    <t>10. controleren van de broncode op aanwezigheid bekende kwetsbare constructies, Bij ICTU: Checkmarx,</t>
+  </si>
+  <si>
+    <t>11. testen op toegankelijkheid van de applicatie. Bij ICTU: Axe.</t>
   </si>
   <si>
     <t>M17</t>
@@ -1400,7 +1405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
@@ -2000,21 +2005,21 @@
       <c r="D67" s="5"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="6"/>
+      <c r="B68" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="C68" s="7"/>
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C68" s="4"/>
-      <c r="D68" s="5"/>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C69" s="7"/>
+      <c r="C69" s="4"/>
       <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:4">
@@ -2034,54 +2039,62 @@
       <c r="D71" s="5"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="6"/>
+      <c r="B72" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B72" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C72" s="4"/>
+      <c r="C72" s="7"/>
       <c r="D72" s="5"/>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="C73" s="4"/>
       <c r="D73" s="5"/>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="C74" s="4"/>
       <c r="D74" s="5"/>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="C75" s="4"/>
       <c r="D75" s="5"/>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="C76" s="4"/>
       <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C77" s="4"/>
+      <c r="D77" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2090,7 +2103,7 @@
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="A51:D51"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C78">
+  <conditionalFormatting sqref="C3:C79">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2105,7 +2118,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C78">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C79">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2130,7 +2143,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2138,10 +2151,10 @@
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>

</xml_diff>